<commit_message>
Added test cases for 2.8 V of VddTest
</commit_message>
<xml_diff>
--- a/docs/best_condition.xlsx
+++ b/docs/best_condition.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>Relazione Dinamica del Segnale / Differenza tra Tensioni</t>
   </si>
@@ -40,6 +40,84 @@
   </si>
   <si>
     <t>DeltaTensione</t>
+  </si>
+  <si>
+    <t>VDDTest</t>
+  </si>
+  <si>
+    <t>Vrif4</t>
+  </si>
+  <si>
+    <t>Delta Tensione</t>
+  </si>
+  <si>
+    <t>HighLight</t>
+  </si>
+  <si>
+    <t>LowLight</t>
+  </si>
+  <si>
+    <t>Dinamica</t>
+  </si>
+  <si>
+    <t>Misura #1</t>
+  </si>
+  <si>
+    <t>Misura #2</t>
+  </si>
+  <si>
+    <t>VddTest</t>
+  </si>
+  <si>
+    <t>2.8 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRif4 </t>
+  </si>
+  <si>
+    <t>2.5 V - 3.1 V</t>
+  </si>
+  <si>
+    <t>Misura #3</t>
+  </si>
+  <si>
+    <t>2.0 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.7 V - 2.3 V </t>
+  </si>
+  <si>
+    <t>Misura #4</t>
+  </si>
+  <si>
+    <t>1,6 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3 V - 1.9 V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONDIZIONI: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorgente luminosa tra LOW e HIGH, ruota di filtri su 6 (ruota scura) e 2 (ruota chiara) </t>
+  </si>
+  <si>
+    <t>2.5 V</t>
+  </si>
+  <si>
+    <t>VRif4</t>
+  </si>
+  <si>
+    <t>2.0 V - 3.0 V</t>
+  </si>
+  <si>
+    <t>Misura #5</t>
+  </si>
+  <si>
+    <t>2,5 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2 V - 2.8 V </t>
   </si>
 </sst>
 </file>
@@ -118,7 +196,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.2507384076990376"/>
           <c:y val="0.12061014919554154"/>
-          <c:w val="0.63859492563429598"/>
+          <c:w val="0.6385949256342961"/>
           <c:h val="0.73066605401115314"/>
         </c:manualLayout>
       </c:layout>
@@ -182,11 +260,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="141838592"/>
-        <c:axId val="141865344"/>
+        <c:axId val="128480384"/>
+        <c:axId val="128482688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141838592"/>
+        <c:axId val="128480384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -213,14 +291,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141865344"/>
+        <c:crossAx val="128482688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.30000000000000016"/>
+        <c:majorUnit val="0.30000000000000021"/>
         <c:minorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141865344"/>
+        <c:axId val="128482688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -246,7 +324,393 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141838592"/>
+        <c:crossAx val="128480384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="4"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$93:$C$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.4000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.50000000000000089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$93:$D$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>34043</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>604530</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>135995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8658</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8064</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6659</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5676</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4423</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3208</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1887</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>853</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="54099328"/>
+        <c:axId val="54097792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="54099328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54097792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54097792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54099328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="13"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$93:$C$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.4000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.50000000000000089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$93:$E$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>34016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>581641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>745440</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86116</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65326</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>54450</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36659</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23465</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8282</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="130630784"/>
+        <c:axId val="82626816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="130630784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82626816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="82626816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="130630784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$144:$C$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$144:$F$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1143149383073998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.753969056527453</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1541844838118518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9323909854647283</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7818897637795281</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.2443015780245474</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0543156762570582</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="81424768"/>
+        <c:axId val="81426304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="81424768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81426304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="81426304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81424768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -256,6 +720,799 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="4"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$144:$C$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$144:$D$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>620820</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9889</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8185</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6350</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5133</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3719</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="90214400"/>
+        <c:axId val="90215936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="90214400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90215936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="90215936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90214400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="13"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$144:$C$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$144:$E$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>691789</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>511795</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74927</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74483</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62115</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>47451</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="90231168"/>
+        <c:axId val="90232704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="90231168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90232704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="90232704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90231168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$193:$C$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$193:$F$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1920464343882733</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.899018360298129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.518798889730002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.5481447408770315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2110963328899871</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1490396927016651</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4859985261606488</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="145060992"/>
+        <c:axId val="145062528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="145060992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.30000000000000004"/>
+          <c:min val="-0.30000000000000004"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="145062528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="145062528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="145060992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="4"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$193:$C$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$193:$D$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>626260</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6522</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5263</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3905</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2714</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="147225984"/>
+        <c:axId val="149972096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="147225984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="149972096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="149972096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="147225984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="13"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$193:$C$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$193:$E$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>746531</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>372957</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75446</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62273</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48478</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31822</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17603</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="89217280"/>
+        <c:axId val="90193920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="89217280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90193920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="90193920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89217280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$239:$C$245</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999867E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000031</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.2000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000049</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$239:$F$245</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2496691492660437</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.977522888591707</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.2340261739799843</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.399860310808451</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.295707762557077</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6972270796902329</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6110937986911811</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="90361216"/>
+        <c:axId val="90416640"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="90361216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.30000000000000016"/>
+          <c:min val="-0.30000000000000016"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90416640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="90416640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90361216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="4"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$193:$C$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$193:$D$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>626260</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6522</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5263</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3905</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2714</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="144592896"/>
+        <c:axId val="144594816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="144592896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144594816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="144594816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144592896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -293,7 +1550,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.2507384076990376"/>
           <c:y val="0.12061014919554154"/>
-          <c:w val="0.63859492563429643"/>
+          <c:w val="0.63859492563429654"/>
           <c:h val="0.73066605401115314"/>
         </c:manualLayout>
       </c:layout>
@@ -415,11 +1672,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="129406848"/>
-        <c:axId val="141836672"/>
+        <c:axId val="129007616"/>
+        <c:axId val="129009536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="129406848"/>
+        <c:axId val="129007616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -446,14 +1703,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141836672"/>
+        <c:crossAx val="129009536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.30000000000000016"/>
+        <c:majorUnit val="0.30000000000000021"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141836672"/>
+        <c:axId val="129009536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,7 +1736,119 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129406848"/>
+        <c:crossAx val="129007616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="13"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$193:$C$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$239:$E$245</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1067986</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>718917</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95960</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>59560</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56369</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34815</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24424</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="144615296"/>
+        <c:axId val="144616832"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="144615296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144616832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="144616832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="144615296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -489,6 +1858,812 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$284:$C$290</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$284:$F$290</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.95409281516469469</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.358088658606793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.289851632047478</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7087443348440416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4975992317541618</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8687388635913678</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.9851498276319282</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="98448512"/>
+        <c:axId val="98450048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="98448512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.30000000000000027"/>
+          <c:min val="-0.30000000000000027"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98450048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="98450048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98448512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="4"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$193:$C$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$284:$D$290</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>641490</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22581</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7502</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6248</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5051</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3771</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="98876032"/>
+        <c:axId val="152436736"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="98876032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152436736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="152436736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98876032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:style val="13"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$239:$C$245</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999867E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000031</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.2000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000049</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$284:$E$290</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>612041</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>685516</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86692</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72835</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59341</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44796</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="152885888"/>
+        <c:axId val="152887680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="152885888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152887680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="152887680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152885888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Comparazione</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> Dinamica Vs Delta Tensione</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3430035388798544E-2"/>
+          <c:y val="8.5252189698463252E-2"/>
+          <c:w val="0.86689067994535485"/>
+          <c:h val="0.80642955982348996"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>2.8 V</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$144:$C$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$144:$F$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1143149383073998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51.753969056527453</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1541844838118518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9323909854647283</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7818897637795281</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.2443015780245474</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0543156762570582</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2.5 V</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$144:$C$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$284:$F$290</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.95409281516469469</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.358088658606793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.289851632047478</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7087443348440416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4975992317541618</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8687388635913678</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.9851498276319282</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2.0 V</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$193:$C$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$193:$F$199</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1920464343882733</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.899018360298129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.518798889730002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.5481447408770315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2110963328899871</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1490396927016651</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4859985261606488</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>1.6 V</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$239:$C$245</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9999999999999867E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.10000000000000031</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.2000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.30000000000000049</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$239:$F$245</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2496691492660437</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.977522888591707</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.2340261739799843</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.399860310808451</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.295707762557077</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6972270796902329</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6110937986911811</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="152568576"/>
+        <c:axId val="152529920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="152568576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>VDDTest - Vrif4</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152529920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="152529920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1800"/>
+                  <a:t>HighLight</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1800" baseline="0"/>
+                  <a:t> / LowLight</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.5405795399342979E-2"/>
+              <c:y val="0.32854586281313702"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152568576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.9138170156355856E-2"/>
+          <c:y val="0.16945247477900563"/>
+          <c:w val="0.29638795101131793"/>
+          <c:h val="0.38093440247588917"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -598,11 +2773,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="90108288"/>
-        <c:axId val="93487104"/>
+        <c:axId val="129021440"/>
+        <c:axId val="129023360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90108288"/>
+        <c:axId val="129021440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -629,14 +2804,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93487104"/>
+        <c:crossAx val="129023360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.30000000000000027"/>
+        <c:majorUnit val="0.30000000000000032"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93487104"/>
+        <c:axId val="129023360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,7 +2837,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90108288"/>
+        <c:crossAx val="129021440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -671,7 +2846,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -773,11 +2948,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="90084480"/>
-        <c:axId val="90260224"/>
+        <c:axId val="129076224"/>
+        <c:axId val="129086592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90084480"/>
+        <c:axId val="129076224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -804,14 +2979,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90260224"/>
+        <c:crossAx val="129086592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.30000000000000027"/>
+        <c:majorUnit val="0.30000000000000032"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90260224"/>
+        <c:axId val="129086592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +3012,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90084480"/>
+        <c:crossAx val="129076224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -846,7 +3021,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -948,11 +3123,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="143637888"/>
-        <c:axId val="143675776"/>
+        <c:axId val="130433792"/>
+        <c:axId val="130435712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="143637888"/>
+        <c:axId val="130433792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -979,14 +3154,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143675776"/>
+        <c:crossAx val="130435712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.30000000000000027"/>
+        <c:majorUnit val="0.30000000000000032"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143675776"/>
+        <c:axId val="130435712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,7 +3187,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143637888"/>
+        <c:crossAx val="130433792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1021,7 +3196,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1093,11 +3268,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="90110208"/>
-        <c:axId val="93475200"/>
+        <c:axId val="130447616"/>
+        <c:axId val="130482560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90110208"/>
+        <c:axId val="130447616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -1124,14 +3299,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93475200"/>
+        <c:crossAx val="130482560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.30000000000000032"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93475200"/>
+        <c:axId val="130482560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1157,7 +3332,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90110208"/>
+        <c:crossAx val="130447616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1166,7 +3341,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1256,11 +3431,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="87425408"/>
-        <c:axId val="87210624"/>
+        <c:axId val="130519040"/>
+        <c:axId val="130520576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87425408"/>
+        <c:axId val="130519040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -1269,14 +3444,14 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87210624"/>
+        <c:crossAx val="130520576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.30000000000000004"/>
+        <c:majorUnit val="0.3000000000000001"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87210624"/>
+        <c:axId val="130520576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,7 +3459,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87425408"/>
+        <c:crossAx val="130519040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1297,7 +3472,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1470,11 +3645,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="143676544"/>
-        <c:axId val="143672832"/>
+        <c:axId val="130536192"/>
+        <c:axId val="130538112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="143676544"/>
+        <c:axId val="130536192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -1509,14 +3684,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143672832"/>
+        <c:crossAx val="130538112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
-        <c:minorUnit val="4.0000000000000008E-2"/>
+        <c:minorUnit val="4.0000000000000015E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143672832"/>
+        <c:axId val="130538112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1546,14 +3721,151 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.8328611898016998E-2"/>
-              <c:y val="0.34814504765851639"/>
+              <c:x val="2.8328611898016994E-2"/>
+              <c:y val="0.34814504765851634"/>
             </c:manualLayout>
           </c:layout>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143676544"/>
+        <c:crossAx val="130536192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="it-IT"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$93:$C$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9999999999999645E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.10000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.20000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.30000000000000071</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.4000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.50000000000000089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$93:$F$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.99920688540962899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96213752832779187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4813779918379355</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9464079464079465</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6865079365079367</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8101817089653096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.5930232558139537</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2882658828849198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.3145261845386536</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3889772125066244</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0562719812426731</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="147138048"/>
+        <c:axId val="147136512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="147138048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="147136512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="147136512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="147138048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1805,6 +4117,486 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>212</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="19" name="Chart 18"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="Chart 19"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="21" name="Chart 20"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>257</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="22" name="Chart 21"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="23" name="Chart 22"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="24" name="Chart 23"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>292</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="25" name="Chart 24"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>305</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="26" name="Chart 25"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="27" name="Chart 26"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>46166</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>58316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>48597</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>155510</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="28" name="Chart 27"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2098,10 +4890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="E103" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="S138" sqref="S138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3133,7 +5925,7 @@
         <v>1.6</v>
       </c>
       <c r="B47">
-        <f t="shared" ref="B47:B49" si="12">B46-0.05</f>
+        <f t="shared" ref="B47:B48" si="12">B46-0.05</f>
         <v>1.95</v>
       </c>
       <c r="C47">
@@ -3179,11 +5971,11 @@
         <v>1.6</v>
       </c>
       <c r="B49">
-        <f>B48-0.05</f>
+        <f t="shared" ref="B49:B62" si="14">B48-0.05</f>
         <v>1.8499999999999999</v>
       </c>
       <c r="C49">
-        <f t="shared" ref="C49:C62" si="14">B49-A49</f>
+        <f t="shared" ref="C49:C62" si="15">B49-A49</f>
         <v>0.24999999999999978</v>
       </c>
       <c r="D49">
@@ -3193,7 +5985,7 @@
         <v>151</v>
       </c>
       <c r="F49">
-        <f t="shared" ref="F49:F62" si="15">D49/E49</f>
+        <f t="shared" ref="F49:F62" si="16">D49/E49</f>
         <v>6826.8940397350989</v>
       </c>
     </row>
@@ -3202,11 +5994,11 @@
         <v>1.6</v>
       </c>
       <c r="B50">
-        <f>B49-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="C50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="D50">
@@ -3216,7 +6008,7 @@
         <v>127</v>
       </c>
       <c r="F50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8302.929133858268</v>
       </c>
     </row>
@@ -3225,11 +6017,11 @@
         <v>1.6</v>
       </c>
       <c r="B51">
-        <f>B50-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.7499999999999998</v>
       </c>
       <c r="C51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.14999999999999969</v>
       </c>
       <c r="D51">
@@ -3239,7 +6031,7 @@
         <v>100</v>
       </c>
       <c r="F51">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>10578.36</v>
       </c>
     </row>
@@ -3248,11 +6040,11 @@
         <v>1.6</v>
       </c>
       <c r="B52">
-        <f>B51-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.6999999999999997</v>
       </c>
       <c r="C52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9.9999999999999645E-2</v>
       </c>
       <c r="D52">
@@ -3262,7 +6054,7 @@
         <v>80</v>
       </c>
       <c r="F52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>13101.4625</v>
       </c>
     </row>
@@ -3271,11 +6063,11 @@
         <v>1.6</v>
       </c>
       <c r="B53">
-        <f>B52-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.6499999999999997</v>
       </c>
       <c r="C53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.99999999999996E-2</v>
       </c>
       <c r="D53">
@@ -3285,7 +6077,7 @@
         <v>61</v>
       </c>
       <c r="F53">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>17148.934426229509</v>
       </c>
     </row>
@@ -3294,11 +6086,11 @@
         <v>1.6</v>
       </c>
       <c r="B54">
-        <f>B53-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.5999999999999996</v>
       </c>
       <c r="C54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="D54">
@@ -3308,7 +6100,7 @@
         <v>52</v>
       </c>
       <c r="F54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>19973.26923076923</v>
       </c>
     </row>
@@ -3317,11 +6109,11 @@
         <v>1.6</v>
       </c>
       <c r="B55">
-        <f>B54-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.5499999999999996</v>
       </c>
       <c r="C55">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-5.0000000000000488E-2</v>
       </c>
       <c r="D55">
@@ -3331,7 +6123,7 @@
         <v>46</v>
       </c>
       <c r="F55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>22651.152173913044</v>
       </c>
     </row>
@@ -3340,11 +6132,11 @@
         <v>1.6</v>
       </c>
       <c r="B56">
-        <f>B55-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.4999999999999996</v>
       </c>
       <c r="C56">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.10000000000000053</v>
       </c>
       <c r="D56">
@@ -3354,7 +6146,7 @@
         <v>40</v>
       </c>
       <c r="F56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>25212.7</v>
       </c>
     </row>
@@ -3363,11 +6155,11 @@
         <v>1.6</v>
       </c>
       <c r="B57">
-        <f>B56-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.4499999999999995</v>
       </c>
       <c r="C57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.15000000000000058</v>
       </c>
       <c r="D57">
@@ -3377,7 +6169,7 @@
         <v>36</v>
       </c>
       <c r="F57">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>24857.555555555555</v>
       </c>
     </row>
@@ -3386,11 +6178,11 @@
         <v>1.6</v>
       </c>
       <c r="B58">
-        <f>B57-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.3999999999999995</v>
       </c>
       <c r="C58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.20000000000000062</v>
       </c>
       <c r="D58">
@@ -3400,7 +6192,7 @@
         <v>33</v>
       </c>
       <c r="F58">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>18317.575757575756</v>
       </c>
     </row>
@@ -3409,11 +6201,11 @@
         <v>1.6</v>
       </c>
       <c r="B59">
-        <f>B58-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.3499999999999994</v>
       </c>
       <c r="C59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.25000000000000067</v>
       </c>
       <c r="D59">
@@ -3423,7 +6215,7 @@
         <v>30</v>
       </c>
       <c r="F59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8791.1333333333332</v>
       </c>
     </row>
@@ -3432,11 +6224,11 @@
         <v>1.6</v>
       </c>
       <c r="B60">
-        <f>B59-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.2999999999999994</v>
       </c>
       <c r="C60">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.30000000000000071</v>
       </c>
       <c r="D60">
@@ -3446,7 +6238,7 @@
         <v>26</v>
       </c>
       <c r="F60">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3600</v>
       </c>
     </row>
@@ -3455,11 +6247,11 @@
         <v>1.6</v>
       </c>
       <c r="B61">
-        <f>B60-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.2499999999999993</v>
       </c>
       <c r="C61">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.35000000000000075</v>
       </c>
       <c r="D61">
@@ -3469,7 +6261,7 @@
         <v>23</v>
       </c>
       <c r="F61">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1485</v>
       </c>
     </row>
@@ -3478,11 +6270,11 @@
         <v>1.6</v>
       </c>
       <c r="B62">
-        <f>B61-0.05</f>
+        <f t="shared" si="14"/>
         <v>1.1999999999999993</v>
       </c>
       <c r="C62">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.4000000000000008</v>
       </c>
       <c r="D62">
@@ -3492,8 +6284,1137 @@
         <v>20</v>
       </c>
       <c r="F62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>607.79999999999995</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>29</v>
+      </c>
+      <c r="B90" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93">
+        <v>2.5</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <f>B93-A93</f>
+        <v>0.5</v>
+      </c>
+      <c r="D93">
+        <v>34043</v>
+      </c>
+      <c r="E93">
+        <v>34016</v>
+      </c>
+      <c r="F93">
+        <f>E93/D93</f>
+        <v>0.99920688540962899</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94">
+        <v>2.5</v>
+      </c>
+      <c r="B94">
+        <f>B93-0.1</f>
+        <v>2.9</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:C103" si="17">B94-A94</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="D94">
+        <v>604530</v>
+      </c>
+      <c r="E94">
+        <v>581641</v>
+      </c>
+      <c r="F94">
+        <f t="shared" ref="F94:F103" si="18">E94/D94</f>
+        <v>0.96213752832779187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95">
+        <v>2.5</v>
+      </c>
+      <c r="B95">
+        <f t="shared" ref="B95:B103" si="19">B94-0.1</f>
+        <v>2.8</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="17"/>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="D95">
+        <v>135995</v>
+      </c>
+      <c r="E95">
+        <v>745440</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="18"/>
+        <v>5.4813779918379355</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <v>2.5</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="19"/>
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="17"/>
+        <v>0.19999999999999973</v>
+      </c>
+      <c r="D96">
+        <v>8658</v>
+      </c>
+      <c r="E96">
+        <v>86116</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="18"/>
+        <v>9.9464079464079465</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
+        <v>2.5</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="19"/>
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="17"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="D97">
+        <v>8064</v>
+      </c>
+      <c r="E97">
+        <v>78112</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="18"/>
+        <v>9.6865079365079367</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <v>2.5</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="19"/>
+        <v>2.4999999999999996</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>6659</v>
+      </c>
+      <c r="E98">
+        <v>65326</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="18"/>
+        <v>9.8101817089653096</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <v>2.5</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="19"/>
+        <v>2.3999999999999995</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="17"/>
+        <v>-0.10000000000000053</v>
+      </c>
+      <c r="D99">
+        <v>5676</v>
+      </c>
+      <c r="E99">
+        <v>54450</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="18"/>
+        <v>9.5930232558139537</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <v>2.5</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="19"/>
+        <v>2.2999999999999994</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="17"/>
+        <v>-0.20000000000000062</v>
+      </c>
+      <c r="D100">
+        <v>4423</v>
+      </c>
+      <c r="E100">
+        <v>36659</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="18"/>
+        <v>8.2882658828849198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <v>2.5</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="19"/>
+        <v>2.1999999999999993</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="17"/>
+        <v>-0.30000000000000071</v>
+      </c>
+      <c r="D101">
+        <v>3208</v>
+      </c>
+      <c r="E101">
+        <v>23465</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="18"/>
+        <v>7.3145261845386536</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102">
+        <v>2.5</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="19"/>
+        <v>2.0999999999999992</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="17"/>
+        <v>-0.4000000000000008</v>
+      </c>
+      <c r="D102">
+        <v>1887</v>
+      </c>
+      <c r="E102">
+        <v>8282</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="18"/>
+        <v>4.3889772125066244</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103">
+        <v>2.5</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="19"/>
+        <v>1.9999999999999991</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="17"/>
+        <v>-0.50000000000000089</v>
+      </c>
+      <c r="D103">
+        <v>853</v>
+      </c>
+      <c r="E103">
+        <v>1754</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="18"/>
+        <v>2.0562719812426731</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" t="s">
+        <v>16</v>
+      </c>
+      <c r="B140" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" t="s">
+        <v>18</v>
+      </c>
+      <c r="B141" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" t="s">
+        <v>8</v>
+      </c>
+      <c r="B143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" t="s">
+        <v>10</v>
+      </c>
+      <c r="D143" t="s">
+        <v>11</v>
+      </c>
+      <c r="E143" t="s">
+        <v>12</v>
+      </c>
+      <c r="F143" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144">
+        <v>2.8</v>
+      </c>
+      <c r="B144">
+        <f>A144+3*0.1</f>
+        <v>3.0999999999999996</v>
+      </c>
+      <c r="C144">
+        <f>B144-A144</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="D144">
+        <v>620820</v>
+      </c>
+      <c r="E144">
+        <v>691789</v>
+      </c>
+      <c r="F144">
+        <f>E144/D144</f>
+        <v>1.1143149383073998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145">
+        <v>2.8</v>
+      </c>
+      <c r="B145">
+        <f>B144-0.1</f>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="C145">
+        <f t="shared" ref="C145:C150" si="20">B145-A145</f>
+        <v>0.19999999999999973</v>
+      </c>
+      <c r="D145">
+        <v>9889</v>
+      </c>
+      <c r="E145">
+        <v>511795</v>
+      </c>
+      <c r="F145">
+        <f t="shared" ref="F145:F150" si="21">E145/D145</f>
+        <v>51.753969056527453</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146">
+        <v>2.8</v>
+      </c>
+      <c r="B146">
+        <f t="shared" ref="B146:B150" si="22">B145-0.1</f>
+        <v>2.8999999999999995</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="20"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="D146">
+        <v>8185</v>
+      </c>
+      <c r="E146">
+        <v>74927</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="21"/>
+        <v>9.1541844838118518</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147">
+        <v>2.8</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="22"/>
+        <v>2.7999999999999994</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>7499</v>
+      </c>
+      <c r="E147">
+        <v>74483</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="21"/>
+        <v>9.9323909854647283</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148">
+        <v>2.8</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="22"/>
+        <v>2.6999999999999993</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="20"/>
+        <v>-0.10000000000000053</v>
+      </c>
+      <c r="D148">
+        <v>6350</v>
+      </c>
+      <c r="E148">
+        <v>62115</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="21"/>
+        <v>9.7818897637795281</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149">
+        <v>2.8</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="22"/>
+        <v>2.5999999999999992</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="20"/>
+        <v>-0.20000000000000062</v>
+      </c>
+      <c r="D149">
+        <v>5133</v>
+      </c>
+      <c r="E149">
+        <v>47451</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="21"/>
+        <v>9.2443015780245474</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150">
+        <v>2.8</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="22"/>
+        <v>2.4999999999999991</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="20"/>
+        <v>-0.30000000000000071</v>
+      </c>
+      <c r="D150">
+        <v>3719</v>
+      </c>
+      <c r="E150">
+        <v>29954</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="21"/>
+        <v>8.0543156762570582</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" t="s">
+        <v>16</v>
+      </c>
+      <c r="B189" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" t="s">
+        <v>18</v>
+      </c>
+      <c r="B190" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" t="s">
+        <v>8</v>
+      </c>
+      <c r="B192" t="s">
+        <v>9</v>
+      </c>
+      <c r="C192" t="s">
+        <v>10</v>
+      </c>
+      <c r="D192" t="s">
+        <v>11</v>
+      </c>
+      <c r="E192" t="s">
+        <v>12</v>
+      </c>
+      <c r="F192" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193">
+        <v>2</v>
+      </c>
+      <c r="B193">
+        <f>A193+3*0.1</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C193">
+        <f>B193-A193</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="D193">
+        <v>626260</v>
+      </c>
+      <c r="E193">
+        <v>746531</v>
+      </c>
+      <c r="F193">
+        <f>E193/D193</f>
+        <v>1.1920464343882733</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194">
+        <f>A193</f>
+        <v>2</v>
+      </c>
+      <c r="B194">
+        <f>B193-0.1</f>
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="C194">
+        <f t="shared" ref="C194:C199" si="23">B194-A194</f>
+        <v>0.19999999999999973</v>
+      </c>
+      <c r="D194">
+        <v>11002</v>
+      </c>
+      <c r="E194">
+        <v>372957</v>
+      </c>
+      <c r="F194">
+        <f t="shared" ref="F194:F199" si="24">E194/D194</f>
+        <v>33.899018360298129</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195">
+        <f t="shared" ref="A195:A199" si="25">A194</f>
+        <v>2</v>
+      </c>
+      <c r="B195">
+        <f t="shared" ref="B195:B199" si="26">B194-0.1</f>
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="C195">
+        <f t="shared" si="23"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="D195">
+        <v>7926</v>
+      </c>
+      <c r="E195">
+        <v>75446</v>
+      </c>
+      <c r="F195">
+        <f t="shared" si="24"/>
+        <v>9.518798889730002</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="B196">
+        <f t="shared" si="26"/>
+        <v>1.9999999999999996</v>
+      </c>
+      <c r="C196">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D196">
+        <v>6522</v>
+      </c>
+      <c r="E196">
+        <v>62273</v>
+      </c>
+      <c r="F196">
+        <f t="shared" si="24"/>
+        <v>9.5481447408770315</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="B197">
+        <f t="shared" si="26"/>
+        <v>1.8999999999999995</v>
+      </c>
+      <c r="C197">
+        <f t="shared" si="23"/>
+        <v>-0.10000000000000053</v>
+      </c>
+      <c r="D197">
+        <v>5263</v>
+      </c>
+      <c r="E197">
+        <v>48478</v>
+      </c>
+      <c r="F197">
+        <f t="shared" si="24"/>
+        <v>9.2110963328899871</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="B198">
+        <f t="shared" si="26"/>
+        <v>1.7999999999999994</v>
+      </c>
+      <c r="C198">
+        <f t="shared" si="23"/>
+        <v>-0.20000000000000062</v>
+      </c>
+      <c r="D198">
+        <v>3905</v>
+      </c>
+      <c r="E198">
+        <v>31822</v>
+      </c>
+      <c r="F198">
+        <f t="shared" si="24"/>
+        <v>8.1490396927016651</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
+      <c r="A199">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="B199">
+        <f t="shared" si="26"/>
+        <v>1.6999999999999993</v>
+      </c>
+      <c r="C199">
+        <f t="shared" si="23"/>
+        <v>-0.30000000000000071</v>
+      </c>
+      <c r="D199">
+        <v>2714</v>
+      </c>
+      <c r="E199">
+        <v>17603</v>
+      </c>
+      <c r="F199">
+        <f t="shared" si="24"/>
+        <v>6.4859985261606488</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="A234" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235" t="s">
+        <v>16</v>
+      </c>
+      <c r="B235" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6">
+      <c r="A236" t="s">
+        <v>18</v>
+      </c>
+      <c r="B236" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6">
+      <c r="A238" t="s">
+        <v>8</v>
+      </c>
+      <c r="B238" t="s">
+        <v>9</v>
+      </c>
+      <c r="C238" t="s">
+        <v>10</v>
+      </c>
+      <c r="D238" t="s">
+        <v>11</v>
+      </c>
+      <c r="E238" t="s">
+        <v>12</v>
+      </c>
+      <c r="F238" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239">
+        <v>1.6</v>
+      </c>
+      <c r="B239">
+        <f>A239+3*0.1</f>
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="C239">
+        <f>B239-A239</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D239">
+        <v>854615</v>
+      </c>
+      <c r="E239">
+        <v>1067986</v>
+      </c>
+      <c r="F239">
+        <f>E239/D239</f>
+        <v>1.2496691492660437</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6">
+      <c r="A240">
+        <f>A239</f>
+        <v>1.6</v>
+      </c>
+      <c r="B240">
+        <f>B239-0.1</f>
+        <v>1.8</v>
+      </c>
+      <c r="C240">
+        <f t="shared" ref="C240:C245" si="27">B240-A240</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="D240">
+        <v>19442</v>
+      </c>
+      <c r="E240">
+        <v>718917</v>
+      </c>
+      <c r="F240">
+        <f t="shared" ref="F240:F245" si="28">E240/D240</f>
+        <v>36.977522888591707</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6">
+      <c r="A241">
+        <f t="shared" ref="A241:A245" si="29">A240</f>
+        <v>1.6</v>
+      </c>
+      <c r="B241">
+        <f t="shared" ref="B241:B245" si="30">B240-0.1</f>
+        <v>1.7</v>
+      </c>
+      <c r="C241">
+        <f t="shared" si="27"/>
+        <v>9.9999999999999867E-2</v>
+      </c>
+      <c r="D241">
+        <v>10392</v>
+      </c>
+      <c r="E241">
+        <v>95960</v>
+      </c>
+      <c r="F241">
+        <f t="shared" si="28"/>
+        <v>9.2340261739799843</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
+      <c r="A242">
+        <f t="shared" si="29"/>
+        <v>1.6</v>
+      </c>
+      <c r="B242">
+        <f t="shared" si="30"/>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="C242">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="D242">
+        <v>5727</v>
+      </c>
+      <c r="E242">
+        <v>59560</v>
+      </c>
+      <c r="F242">
+        <f t="shared" si="28"/>
+        <v>10.399860310808451</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6">
+      <c r="A243">
+        <f t="shared" si="29"/>
+        <v>1.6</v>
+      </c>
+      <c r="B243">
+        <f t="shared" si="30"/>
+        <v>1.4999999999999998</v>
+      </c>
+      <c r="C243">
+        <f t="shared" si="27"/>
+        <v>-0.10000000000000031</v>
+      </c>
+      <c r="D243">
+        <v>5475</v>
+      </c>
+      <c r="E243">
+        <v>56369</v>
+      </c>
+      <c r="F243">
+        <f t="shared" si="28"/>
+        <v>10.295707762557077</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
+      <c r="A244">
+        <f t="shared" si="29"/>
+        <v>1.6</v>
+      </c>
+      <c r="B244">
+        <f t="shared" si="30"/>
+        <v>1.3999999999999997</v>
+      </c>
+      <c r="C244">
+        <f t="shared" si="27"/>
+        <v>-0.2000000000000004</v>
+      </c>
+      <c r="D244">
+        <v>4003</v>
+      </c>
+      <c r="E244">
+        <v>34815</v>
+      </c>
+      <c r="F244">
+        <f t="shared" si="28"/>
+        <v>8.6972270796902329</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6">
+      <c r="A245">
+        <f t="shared" si="29"/>
+        <v>1.6</v>
+      </c>
+      <c r="B245">
+        <f t="shared" si="30"/>
+        <v>1.2999999999999996</v>
+      </c>
+      <c r="C245">
+        <f t="shared" si="27"/>
+        <v>-0.30000000000000049</v>
+      </c>
+      <c r="D245">
+        <v>3209</v>
+      </c>
+      <c r="E245">
+        <v>24424</v>
+      </c>
+      <c r="F245">
+        <f t="shared" si="28"/>
+        <v>7.6110937986911811</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6">
+      <c r="A279" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6">
+      <c r="A280" t="s">
+        <v>16</v>
+      </c>
+      <c r="B280" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6">
+      <c r="A281" t="s">
+        <v>18</v>
+      </c>
+      <c r="B281" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6">
+      <c r="A283" t="s">
+        <v>8</v>
+      </c>
+      <c r="B283" t="s">
+        <v>9</v>
+      </c>
+      <c r="C283" t="s">
+        <v>10</v>
+      </c>
+      <c r="D283" t="s">
+        <v>11</v>
+      </c>
+      <c r="E283" t="s">
+        <v>12</v>
+      </c>
+      <c r="F283" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6">
+      <c r="A284">
+        <v>2.5</v>
+      </c>
+      <c r="B284">
+        <f>A284+3*0.1</f>
+        <v>2.8</v>
+      </c>
+      <c r="C284">
+        <f>B284-A284</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="D284">
+        <v>641490</v>
+      </c>
+      <c r="E284">
+        <v>612041</v>
+      </c>
+      <c r="F284">
+        <f>E284/D284</f>
+        <v>0.95409281516469469</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6">
+      <c r="A285">
+        <f>A284</f>
+        <v>2.5</v>
+      </c>
+      <c r="B285">
+        <f>B284-0.1</f>
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="C285">
+        <f t="shared" ref="C285:C290" si="31">B285-A285</f>
+        <v>0.19999999999999973</v>
+      </c>
+      <c r="D285">
+        <v>22581</v>
+      </c>
+      <c r="E285">
+        <v>685516</v>
+      </c>
+      <c r="F285">
+        <f t="shared" ref="F285:F290" si="32">E285/D285</f>
+        <v>30.358088658606793</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6">
+      <c r="A286">
+        <f t="shared" ref="A286:A290" si="33">A285</f>
+        <v>2.5</v>
+      </c>
+      <c r="B286">
+        <f t="shared" ref="B286:B290" si="34">B285-0.1</f>
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="C286">
+        <f t="shared" si="31"/>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="D286">
+        <v>8425</v>
+      </c>
+      <c r="E286">
+        <v>86692</v>
+      </c>
+      <c r="F286">
+        <f t="shared" si="32"/>
+        <v>10.289851632047478</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6">
+      <c r="A287">
+        <f t="shared" si="33"/>
+        <v>2.5</v>
+      </c>
+      <c r="B287">
+        <f t="shared" si="34"/>
+        <v>2.4999999999999996</v>
+      </c>
+      <c r="C287">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="D287">
+        <v>7502</v>
+      </c>
+      <c r="E287">
+        <v>72835</v>
+      </c>
+      <c r="F287">
+        <f t="shared" si="32"/>
+        <v>9.7087443348440416</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6">
+      <c r="A288">
+        <f t="shared" si="33"/>
+        <v>2.5</v>
+      </c>
+      <c r="B288">
+        <f t="shared" si="34"/>
+        <v>2.3999999999999995</v>
+      </c>
+      <c r="C288">
+        <f t="shared" si="31"/>
+        <v>-0.10000000000000053</v>
+      </c>
+      <c r="D288">
+        <v>6248</v>
+      </c>
+      <c r="E288">
+        <v>59341</v>
+      </c>
+      <c r="F288">
+        <f t="shared" si="32"/>
+        <v>9.4975992317541618</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6">
+      <c r="A289">
+        <f t="shared" si="33"/>
+        <v>2.5</v>
+      </c>
+      <c r="B289">
+        <f t="shared" si="34"/>
+        <v>2.2999999999999994</v>
+      </c>
+      <c r="C289">
+        <f t="shared" si="31"/>
+        <v>-0.20000000000000062</v>
+      </c>
+      <c r="D289">
+        <v>5051</v>
+      </c>
+      <c r="E289">
+        <v>44796</v>
+      </c>
+      <c r="F289">
+        <f t="shared" si="32"/>
+        <v>8.8687388635913678</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6">
+      <c r="A290">
+        <f t="shared" si="33"/>
+        <v>2.5</v>
+      </c>
+      <c r="B290">
+        <f t="shared" si="34"/>
+        <v>2.1999999999999993</v>
+      </c>
+      <c r="C290">
+        <f t="shared" si="31"/>
+        <v>-0.30000000000000071</v>
+      </c>
+      <c r="D290">
+        <v>3771</v>
+      </c>
+      <c r="E290">
+        <v>30112</v>
+      </c>
+      <c r="F290">
+        <f t="shared" si="32"/>
+        <v>7.9851498276319282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>